<commit_message>
Bug fixes to get it running again
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12555"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Configuration Testing" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Test</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Go into the LbcbPlugin Folder and double click on the LbcbPlugin code file</t>
+  </si>
+  <si>
+    <t>MATLAB should start up with a command window and an editor window</t>
+  </si>
+  <si>
+    <t>The window should clear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can dismiss the editor window.  Type "clearSpace" in the command window.  </t>
   </si>
 </sst>
 </file>
@@ -459,7 +471,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,18 +502,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>

</xml_diff>

<commit_message>
Test version of ED works again
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,20 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration Testing" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Plugin+OM Testing" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>Test</t>
   </si>
@@ -43,10 +42,208 @@
     <t>MATLAB should start up with a command window and an editor window</t>
   </si>
   <si>
-    <t>The window should clear.</t>
-  </si>
-  <si>
     <t xml:space="preserve">You can dismiss the editor window.  Type "clearSpace" in the command window.  </t>
+  </si>
+  <si>
+    <t>The command window should clear.</t>
+  </si>
+  <si>
+    <t>Type "LbcbPlugin" in the command window</t>
+  </si>
+  <si>
+    <t>The LbcbPlugin should start up.  Report any red errors</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Network Configuration</t>
+  </si>
+  <si>
+    <t>Enter unique values for each field and click on 'OK'</t>
+  </si>
+  <si>
+    <t>The Network Configuration window should disappear</t>
+  </si>
+  <si>
+    <t>The Network Configuration window should appear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Network Configuration again</t>
+  </si>
+  <si>
+    <t>Verify that the unique values are still there</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;OM Configuration</t>
+  </si>
+  <si>
+    <t>The OM Configuration window should appear</t>
+  </si>
+  <si>
+    <t>Enter unique values for each field</t>
+  </si>
+  <si>
+    <t>Click on the + button to add a new sensor add several sensors with unique values</t>
+  </si>
+  <si>
+    <t>The '+' button should create a new entry right above the selected sensor</t>
+  </si>
+  <si>
+    <t>Skip the sensor table.</t>
+  </si>
+  <si>
+    <t>Click on the '^' and 'v' buttons to move the selected sensor</t>
+  </si>
+  <si>
+    <t>Make sure that the sensor is moving up and down as directed by the buttons that were clicked</t>
+  </si>
+  <si>
+    <t>Select a sensor row and click '-'</t>
+  </si>
+  <si>
+    <t>The sensor row should be removed</t>
+  </si>
+  <si>
+    <t>Click 'OK'</t>
+  </si>
+  <si>
+    <t>The OM Configuration window should disappear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;OM Configuration again</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Step Configuration</t>
+  </si>
+  <si>
+    <t>The Step Configuration window should appear</t>
+  </si>
+  <si>
+    <t>The Step Configuration window should disappear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Step Configuration again</t>
+  </si>
+  <si>
+    <t>The Correction Settings window should appear</t>
+  </si>
+  <si>
+    <t>The Correction Settings window should disappear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Correction Settings again</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Correction Settings</t>
+  </si>
+  <si>
+    <t>Enter unique labels and values for the first 4 rows  and click on 'OK'</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Target Configuration</t>
+  </si>
+  <si>
+    <t>The Target Configuration window should appear</t>
+  </si>
+  <si>
+    <t>The Target Configuration window should disappear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Target Configuration again</t>
+  </si>
+  <si>
+    <t>Skip the control point address table.</t>
+  </si>
+  <si>
+    <t>Click on the '^' and 'v' buttons to move the selected control point address</t>
+  </si>
+  <si>
+    <t>Select a control point address row and click '-'</t>
+  </si>
+  <si>
+    <t>Click on the + button to add a new control point address add several control point addresses with unique values</t>
+  </si>
+  <si>
+    <t>Select a control point address row and click 'e'</t>
+  </si>
+  <si>
+    <t>A popup should allow you to edit the address</t>
+  </si>
+  <si>
+    <t>The '+' button should create a new entry right above the selected address</t>
+  </si>
+  <si>
+    <t>Make sure that the address is moving up and down as directed by the buttons that were clicked</t>
+  </si>
+  <si>
+    <t>The  address should be removed</t>
+  </si>
+  <si>
+    <t>The Logging Levels window should appear</t>
+  </si>
+  <si>
+    <t>The Logging Levels window should disappear</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Logging Levels again</t>
+  </si>
+  <si>
+    <t>Select Edit-&gt;Logging Levels</t>
+  </si>
+  <si>
+    <t>Select File-&gt;Save</t>
+  </si>
+  <si>
+    <t>Restart the LbcbPlugin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check all of the edit windows again </t>
+  </si>
+  <si>
+    <t>All of the values you entered should still be there</t>
+  </si>
+  <si>
+    <t>Configuration Test</t>
+  </si>
+  <si>
+    <t>Open a Cmd window on the OM system and type 'ipconfig /all'</t>
+  </si>
+  <si>
+    <t>Record the IP address of the system.  It should be something like cee-nees****.cee.illinois.edu</t>
+  </si>
+  <si>
+    <t>Start the OM in accordance with the Operation Manager startup procedure.  Autobalance the LBCB.  Turn the control on.  Check to see if your displacements and commands are relatively the same.  Turn on the oil pressure.</t>
+  </si>
+  <si>
+    <t>Switch over to the NTCP window and click on connect to server.</t>
+  </si>
+  <si>
+    <t>This is the point where you can restart the LbcbPlugin test.  When the LbcbPlugin exits,  the NTCP socket window disappears.  Before restarting the plugin,  click on the connect to server button to restore this window</t>
+  </si>
+  <si>
+    <t>If your LBCB is not connected to a specimen then apply "Reset Targets to Zero" and run a manual ramp.  If you are connected to a specimen then set the command and displacement offsets and  switch to "Local" coordinates</t>
+  </si>
+  <si>
+    <t>OM Startup</t>
+  </si>
+  <si>
+    <t>Open the LbcbPlugin folder on the desktop and double click on the LbcbPlugin code file (not the .fig file!)</t>
+  </si>
+  <si>
+    <t>MATLAB should display a command window and an editor window</t>
+  </si>
+  <si>
+    <t>Get rid of the edit window</t>
+  </si>
+  <si>
+    <t>In the command window type 'clearSpace' and hit return</t>
+  </si>
+  <si>
+    <t>A bunch of messages will be displayed.  In general, report any messages that use red lettering</t>
+  </si>
+  <si>
+    <t>Type 'LbcbPlugin' in the command window</t>
+  </si>
+  <si>
+    <t>The LbcbPlugin main window should appear.</t>
   </si>
 </sst>
 </file>
@@ -142,15 +339,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -158,13 +352,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -468,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,86 +708,403 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A34"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -590,12 +1112,119 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58" style="13" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Test matrix and fixes
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Configuration Testing" sheetId="1" r:id="rId1"/>
-    <sheet name="Plugin+OM Testing" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Configuration Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Basic Test" sheetId="4" r:id="rId2"/>
+    <sheet name="ED Test" sheetId="5" r:id="rId3"/>
+    <sheet name="DD Test" sheetId="7" r:id="rId4"/>
+    <sheet name="Startup" sheetId="2" r:id="rId5"/>
+    <sheet name="Basic Setup" sheetId="3" r:id="rId6"/>
+    <sheet name="ED Setup" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
   <si>
     <t>Test</t>
   </si>
@@ -210,21 +214,12 @@
     <t>Record the IP address of the system.  It should be something like cee-nees****.cee.illinois.edu</t>
   </si>
   <si>
-    <t>Start the OM in accordance with the Operation Manager startup procedure.  Autobalance the LBCB.  Turn the control on.  Check to see if your displacements and commands are relatively the same.  Turn on the oil pressure.</t>
-  </si>
-  <si>
     <t>Switch over to the NTCP window and click on connect to server.</t>
   </si>
   <si>
     <t>This is the point where you can restart the LbcbPlugin test.  When the LbcbPlugin exits,  the NTCP socket window disappears.  Before restarting the plugin,  click on the connect to server button to restore this window</t>
   </si>
   <si>
-    <t>If your LBCB is not connected to a specimen then apply "Reset Targets to Zero" and run a manual ramp.  If you are connected to a specimen then set the command and displacement offsets and  switch to "Local" coordinates</t>
-  </si>
-  <si>
-    <t>OM Startup</t>
-  </si>
-  <si>
     <t>Open the LbcbPlugin folder on the desktop and double click on the LbcbPlugin code file (not the .fig file!)</t>
   </si>
   <si>
@@ -244,13 +239,205 @@
   </si>
   <si>
     <t>The LbcbPlugin main window should appear.</t>
+  </si>
+  <si>
+    <t>Start OM Setup and check in the timing and logging window for the NTCP Network values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  None of the fields should be blank or zero.  Record the port number so that you can verify it in the LbcbPlugin configuration</t>
+  </si>
+  <si>
+    <t>Start the OM in accordance with the Operation Manager startup procedure.  Autobalance the LBCB.  Turn the control on.  Check to see if your displacements and commands are relatively the same.  You can turn on the  oil pressure if the LBCB(s) are free.</t>
+  </si>
+  <si>
+    <t>Start Up</t>
+  </si>
+  <si>
+    <t>No Step Splitting</t>
+  </si>
+  <si>
+    <t>No Substep Correction</t>
+  </si>
+  <si>
+    <t>No Substep Triggering</t>
+  </si>
+  <si>
+    <t>No Elastic Deformation Calculation or Correction</t>
+  </si>
+  <si>
+    <t>No Derived DOF Calculation or Correction</t>
+  </si>
+  <si>
+    <t>No Preliminary Adjustment</t>
+  </si>
+  <si>
+    <t>Command and Increment Limits are clear</t>
+  </si>
+  <si>
+    <t>Step Tolerances are clear</t>
+  </si>
+  <si>
+    <t>External Sensors match in name and order to the OM</t>
+  </si>
+  <si>
+    <t>Run the Startup procedure and set up the Basic Setup</t>
+  </si>
+  <si>
+    <t>Apply "Reset Targets to Zero" and run a manual ramp.</t>
+  </si>
+  <si>
+    <t>Open Edit-&gt;Network Configuration and make sure that the OM link hostname and port are correct.</t>
+  </si>
+  <si>
+    <t>Press the OM button</t>
+  </si>
+  <si>
+    <t>Button should turn green. The NTCP window on the OM should indicate that it is waiting for messages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press the manual button LbcbPlugin and both manual buttons on the OM. </t>
+  </si>
+  <si>
+    <t>All of the buttons should switch to Auto.  This is not a good idea for a real test.  However it speeds this testing up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The message window will show that 13 steps were loaded </t>
+  </si>
+  <si>
+    <t>The message window will indicate that the OM is connected</t>
+  </si>
+  <si>
+    <t>Press the Input File button and select the file DxDyRx in the InputFiles folder</t>
+  </si>
+  <si>
+    <t>A separate popup table should appear with twelve DOFs as column headers</t>
+  </si>
+  <si>
+    <t>Press Run</t>
+  </si>
+  <si>
+    <t>The message window will show 13 steps being executed.  The command window will show the 13 commands</t>
+  </si>
+  <si>
+    <t>Compare the command window numbers with the DxDyRx.txt file</t>
+  </si>
+  <si>
+    <t>The three columns in this file should match the Dx, Dy, and Rx columns in the command table.</t>
+  </si>
+  <si>
+    <t>Open View-&gt;Tables-&gt;LBCB1 Command Table</t>
+  </si>
+  <si>
+    <t>In Edit-&gt;Step Configuration Enable step splitting and enter the following increments: Dx=0.25, Dy=0.1, Rx = 5e-6</t>
+  </si>
+  <si>
+    <t>Two substeps will be executed for every step except step 9 which will have 8 substeps.</t>
+  </si>
+  <si>
+    <t>Change the step increment for Rx to 1e-5 and resume the test by pressing Run again</t>
+  </si>
+  <si>
+    <t>Steps 10 through 13 will have 4 substeps.</t>
+  </si>
+  <si>
+    <t>Disable step splitting</t>
+  </si>
+  <si>
+    <t>Reload the DxDyRx file and press Run.  At Step 9 press hold to pause the test</t>
+  </si>
+  <si>
+    <t>Open Edit-&gt;Command Limits and enter -0.4 and + 0.4 as the command limits for Dx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reload the DxDyRx file and press Run.  </t>
+  </si>
+  <si>
+    <t>Increase the limit to +0.6 and press Run</t>
+  </si>
+  <si>
+    <t>The test will stop again and complain about Dx exceeding the lower limit.</t>
+  </si>
+  <si>
+    <t>Both upper and lower limits for DX will be blank.  The test will finish.</t>
+  </si>
+  <si>
+    <t>Remove the lower Dx limit and press Run.</t>
+  </si>
+  <si>
+    <t>Results should be the same</t>
+  </si>
+  <si>
+    <t>Open Edit-&gt;Increment Limits and set the Dx limit to 0.4</t>
+  </si>
+  <si>
+    <t>Reload the DxDyRx file and press Run</t>
+  </si>
+  <si>
+    <t>The test will stop at step 1.  The Run button will be yellow.  The alert box will show that Dx exceeded a limit.  The Auto button will be switched to manual</t>
+  </si>
+  <si>
+    <t>Press Edit and change the Dx target to 0.37.  Press the Run button and the Accept button.</t>
+  </si>
+  <si>
+    <t>The test will pause again when the commanded Dx is -0.4.</t>
+  </si>
+  <si>
+    <t>Repeat the command limits test steps for Dy = +/- 0.17 and Rx = +/- 3e-5</t>
+  </si>
+  <si>
+    <t>Clear the increment limit and press Run</t>
+  </si>
+  <si>
+    <t>The test will finish.</t>
+  </si>
+  <si>
+    <t>Repeat the increment limits test steps for Dy =  0.17 and Rx = 3e-5</t>
+  </si>
+  <si>
+    <t>Basic Test</t>
+  </si>
+  <si>
+    <t>Run the Startup procedure and set up the ED Setup</t>
+  </si>
+  <si>
+    <t>Both Elastic Deformation Calculation and Correction are set</t>
+  </si>
+  <si>
+    <t>Step Tolerances for Dx is set to 0.001</t>
+  </si>
+  <si>
+    <t>The message window will show 13 steps being executed.  Each step will have 3 correction steps due to a deliberate mis-calculation in the ED test function.  Notice that the step tolerance will show that the Dx value is out of tolerance for all but the last correction step.  Note also that this out-of-tolerance value is used to adjust the next correction command.</t>
+  </si>
+  <si>
+    <t>In Edit-&gt;Step Configuration Enable step splitting and enter the following increments: Dx=0.25, Dy=0.1, Rx = 5e-6.  Enable substep correction and set to correct every 2 substeps.</t>
+  </si>
+  <si>
+    <t>Two substeps will be executed for every step except step 9 which will have 8 substeps.  Every even substep will have 3 correction steps generated</t>
+  </si>
+  <si>
+    <t>The test will stop at the step 2 substep 2.  The Run button will be yellow.  The alert box will show that Dx has exceeded a limit.  The Auto button will have switched to Manual.</t>
+  </si>
+  <si>
+    <t>The test will stop at the step 1 substep 2 mostlikely at a correction step.  The Run button will be yellow.  The alert box will show that Dx has exceeded a limit.  The Auto button will have switched to Manual.</t>
+  </si>
+  <si>
+    <t>Elastic Deformation  Test</t>
+  </si>
+  <si>
+    <t>Set the elastic Deformation Preliminary Adjustment to 'Test'</t>
+  </si>
+  <si>
+    <t>Reload the DxDyRx file and press Run.  Open the Derived Data Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Derived Data Table should show correction deltas for each step </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +449,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -355,6 +550,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -366,12 +564,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,6 +592,104 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5314950" y="0"/>
+          <a:ext cx="10058400" cy="6705600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>8356</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5314950" y="8356"/>
+          <a:ext cx="10058400" cy="6697238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,7 +982,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +1014,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -722,7 +1028,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -734,7 +1040,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -746,7 +1052,7 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -758,7 +1064,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -770,7 +1076,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
@@ -782,7 +1088,7 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -794,7 +1100,7 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
@@ -806,7 +1112,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -818,7 +1124,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
@@ -830,7 +1136,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
@@ -842,7 +1148,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
@@ -854,7 +1160,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
@@ -866,7 +1172,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
@@ -878,7 +1184,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
@@ -890,7 +1196,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -902,7 +1208,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
@@ -914,7 +1220,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -926,7 +1232,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
@@ -938,7 +1244,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
@@ -950,7 +1256,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -962,7 +1268,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -974,7 +1280,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
@@ -986,7 +1292,7 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
@@ -998,7 +1304,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -1010,7 +1316,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="6" t="s">
         <v>28</v>
       </c>
@@ -1022,7 +1328,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="6" t="s">
         <v>43</v>
       </c>
@@ -1034,7 +1340,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="5" t="s">
         <v>56</v>
       </c>
@@ -1046,7 +1352,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="5" t="s">
         <v>39</v>
       </c>
@@ -1058,7 +1364,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1070,7 +1376,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
         <v>57</v>
       </c>
@@ -1080,7 +1386,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="6" t="s">
         <v>58</v>
       </c>
@@ -1090,7 +1396,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="6" t="s">
         <v>59</v>
       </c>
@@ -1112,18 +1418,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58" style="13" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1147,83 +1453,230 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>63</v>
+      <c r="A2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="5"/>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="5"/>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>66</v>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A2:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1231,12 +1684,705 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58" style="7" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reload bug fixed load properties bug fixed DD test written More ED and substep debug statements UI-SimCor link works
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="405" windowWidth="17175" windowHeight="11130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration Test" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="Startup" sheetId="2" r:id="rId5"/>
     <sheet name="Basic Setup" sheetId="3" r:id="rId6"/>
     <sheet name="ED Setup" sheetId="6" r:id="rId7"/>
+    <sheet name="DD Setup" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="142">
   <si>
     <t>Test</t>
   </si>
@@ -431,13 +432,28 @@
   </si>
   <si>
     <t xml:space="preserve">The Derived Data Table should show correction deltas for each step </t>
+  </si>
+  <si>
+    <t>Derived DOF Calculation and  Correction are set for DD0, DD1  and DD2</t>
+  </si>
+  <si>
+    <t>Run the Startup procedure and set up the DD Setup</t>
+  </si>
+  <si>
+    <t>The message window will show 13 steps being executed.  For each step,  the message window will show all 3 DD levels being calculated.  Each level in will be adjusted in a separate correction step.  No two levels will  be adjusted at the same time.  The correction step number will be calcluated to be level^100.  Allowing each correction level to have 99 steps.  The adjustment will be in Dx which will show a 1e-4 difference from the target</t>
+  </si>
+  <si>
+    <t>In Edit-&gt;Step Configuration set Prelim DD Adjust to 'Test'</t>
+  </si>
+  <si>
+    <t>You will notice in the message window that Prelim Adjust is done right before a step is executed.  The adjustment is done on Dx which is modified +/- 9e-4 depending on whether the step number is odd or even.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +473,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -553,23 +575,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -579,7 +596,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,6 +704,55 @@
         <a:xfrm>
           <a:off x="5314950" y="8356"/>
           <a:ext cx="10058400" cy="6697238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>46654</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>8356</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>258146</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5361604" y="8356"/>
+          <a:ext cx="9965092" cy="6697238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1014,7 +1086,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1028,7 +1100,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1040,7 +1112,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1052,7 +1124,7 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1136,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1148,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1160,7 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1172,7 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1112,7 +1184,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1124,7 +1196,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1136,7 +1208,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
@@ -1148,7 +1220,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1160,7 +1232,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
@@ -1172,7 +1244,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
@@ -1184,7 +1256,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1268,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -1208,7 +1280,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
@@ -1220,7 +1292,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -1232,7 +1304,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5" t="s">
         <v>37</v>
       </c>
@@ -1244,7 +1316,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5" t="s">
         <v>40</v>
       </c>
@@ -1256,7 +1328,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1268,7 +1340,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1280,7 +1352,7 @@
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
@@ -1292,7 +1364,7 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
@@ -1304,7 +1376,7 @@
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="6" t="s">
         <v>48</v>
       </c>
@@ -1316,7 +1388,7 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="6" t="s">
         <v>28</v>
       </c>
@@ -1328,7 +1400,7 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="6" t="s">
         <v>43</v>
       </c>
@@ -1340,7 +1412,7 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="5" t="s">
         <v>56</v>
       </c>
@@ -1352,7 +1424,7 @@
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="5" t="s">
         <v>39</v>
       </c>
@@ -1364,7 +1436,7 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1376,7 +1448,7 @@
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="6" t="s">
         <v>57</v>
       </c>
@@ -1386,7 +1458,7 @@
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="6" t="s">
         <v>58</v>
       </c>
@@ -1396,7 +1468,7 @@
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="6" t="s">
         <v>59</v>
       </c>
@@ -1427,8 +1499,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1453,13 +1525,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4"/>
@@ -1467,11 +1539,11 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="D3" s="4"/>
@@ -1479,11 +1551,11 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="4"/>
@@ -1491,11 +1563,11 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D5" s="4"/>
@@ -1503,11 +1575,11 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="9" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="4"/>
@@ -1515,21 +1587,21 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="4"/>
@@ -1537,11 +1609,11 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="9" t="s">
         <v>105</v>
       </c>
       <c r="D9" s="4"/>
@@ -1549,21 +1621,21 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="9" t="s">
         <v>131</v>
       </c>
       <c r="D11" s="4"/>
@@ -1571,11 +1643,11 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="9" t="s">
         <v>111</v>
       </c>
       <c r="D12" s="4"/>
@@ -1583,11 +1655,11 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D13" s="4"/>
@@ -1595,11 +1667,11 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D14" s="4"/>
@@ -1607,31 +1679,31 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="9" t="s">
         <v>117</v>
       </c>
       <c r="D17" s="4"/>
@@ -1639,11 +1711,11 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="9" t="s">
         <v>119</v>
       </c>
       <c r="D18" s="4"/>
@@ -1651,11 +1723,11 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="9" t="s">
         <v>122</v>
       </c>
       <c r="D19" s="4"/>
@@ -1663,11 +1735,11 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D20" s="4"/>
@@ -1686,15 +1758,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1719,13 +1791,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4"/>
@@ -1733,11 +1805,11 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="D3" s="4"/>
@@ -1745,11 +1817,11 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="4"/>
@@ -1757,11 +1829,11 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="9" t="s">
         <v>128</v>
       </c>
       <c r="D5" s="4"/>
@@ -1769,21 +1841,21 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>130</v>
       </c>
       <c r="D7" s="4"/>
@@ -1791,11 +1863,11 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>105</v>
       </c>
       <c r="D8" s="4"/>
@@ -1803,21 +1875,21 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="9" t="s">
         <v>132</v>
       </c>
       <c r="D10" s="4"/>
@@ -1825,11 +1897,11 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="9" t="s">
         <v>111</v>
       </c>
       <c r="D11" s="4"/>
@@ -1837,11 +1909,11 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D12" s="4"/>
@@ -1849,11 +1921,11 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D13" s="4"/>
@@ -1861,21 +1933,21 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="9" t="s">
         <v>136</v>
       </c>
       <c r="D15" s="4"/>
@@ -1892,17 +1964,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1927,13 +1999,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4"/>
@@ -1941,11 +2013,11 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="D3" s="4"/>
@@ -1953,45 +2025,45 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>128</v>
+      <c r="C5" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="9" t="s">
         <v>130</v>
       </c>
       <c r="D7" s="4"/>
@@ -1999,78 +2071,42 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="9" t="s">
         <v>105</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="14"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>132</v>
+      <c r="C10" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A2:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2113,7 +2149,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2127,7 +2163,7 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5" t="s">
         <v>73</v>
       </c>
@@ -2139,7 +2175,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="5" t="s">
         <v>75</v>
       </c>
@@ -2149,7 +2185,7 @@
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>87</v>
       </c>
@@ -2159,7 +2195,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>64</v>
       </c>
@@ -2171,7 +2207,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>66</v>
       </c>
@@ -2183,7 +2219,7 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="5" t="s">
         <v>68</v>
       </c>
@@ -2193,7 +2229,7 @@
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5" t="s">
         <v>69</v>
       </c>
@@ -2205,7 +2241,7 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5" t="s">
         <v>71</v>
       </c>
@@ -2217,7 +2253,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5" t="s">
         <v>88</v>
       </c>
@@ -2227,7 +2263,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5" t="s">
         <v>89</v>
       </c>
@@ -2239,7 +2275,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>91</v>
       </c>
@@ -2352,7 +2388,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2372,7 +2408,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="10" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2385,4 +2421,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>